<commit_message>
training and validation ratio calc
</commit_message>
<xml_diff>
--- a/stat/split/train-val ratio.xlsx
+++ b/stat/split/train-val ratio.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t>N</t>
   </si>
@@ -80,6 +80,51 @@
   </si>
   <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t>Classes</t>
+  </si>
+  <si>
+    <t>p-value</t>
+  </si>
+  <si>
+    <t>constant</t>
+  </si>
+  <si>
+    <t>Largest nb of images in a class</t>
+  </si>
+  <si>
+    <t>size of training database</t>
+  </si>
+  <si>
+    <t>fraction for val</t>
+  </si>
+  <si>
+    <t>fraction for training</t>
+  </si>
+  <si>
+    <t>hmax/t</t>
+  </si>
+  <si>
+    <t>(c(ln(n/alpha^2))/t</t>
+  </si>
+  <si>
+    <t>a * (f / (1-f)</t>
+  </si>
+  <si>
+    <t>b/f</t>
+  </si>
+  <si>
+    <t>d/f of f</t>
+  </si>
+  <si>
+    <t>a+b</t>
+  </si>
+  <si>
+    <t>learning curve + uncertainty</t>
+  </si>
+  <si>
+    <t>f* / g*</t>
   </si>
 </sst>
 </file>
@@ -87,7 +132,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="173" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -134,14 +179,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -195,7 +243,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Blad2!$A$5:$A$6</c:f>
+              <c:f>Blad2!$A$6:$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -209,7 +257,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Blad2!$H$5:$H$6</c:f>
+              <c:f>Blad2!$H$6:$H$7</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="2"/>
@@ -240,7 +288,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Blad2!$A$5:$A$6</c:f>
+              <c:f>Blad2!$A$6:$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -254,7 +302,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Blad2!$G$5:$G$6</c:f>
+              <c:f>Blad2!$G$6:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="2"/>
@@ -278,11 +326,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="58215808"/>
-        <c:axId val="58221696"/>
+        <c:axId val="128291200"/>
+        <c:axId val="128292736"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="58215808"/>
+        <c:axId val="128291200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -291,7 +339,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58221696"/>
+        <c:crossAx val="128292736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -299,7 +347,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="58221696"/>
+        <c:axId val="128292736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -310,7 +358,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58215808"/>
+        <c:crossAx val="128291200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -338,13 +386,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>252411</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>119061</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>342899</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>47624</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -654,27 +702,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q6"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T20" sqref="T20"/>
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" customWidth="1"/>
-    <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.85546875" customWidth="1"/>
-    <col min="16" max="16" width="8.5703125" customWidth="1"/>
-    <col min="17" max="17" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="17" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
@@ -745,76 +781,62 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5">
-        <v>10</v>
-      </c>
-      <c r="C5">
-        <v>0.05</v>
-      </c>
-      <c r="D5">
-        <v>1.5</v>
-      </c>
-      <c r="E5">
-        <v>100</v>
-      </c>
-      <c r="F5">
-        <v>1000</v>
-      </c>
-      <c r="G5" s="1">
-        <f>Q5/(1+Q5)</f>
-        <v>0.26074820721510727</v>
-      </c>
-      <c r="H5" s="1">
-        <f>1-G5</f>
-        <v>0.73925179278489273</v>
-      </c>
-      <c r="I5" s="1">
-        <f>E5/F5</f>
-        <v>0.1</v>
-      </c>
-      <c r="J5" s="1">
-        <f>(D5*LN(B5/(C5^2)))/F5</f>
-        <v>1.2441074460153041E-2</v>
-      </c>
-      <c r="K5" s="1">
-        <f>I5*(G5/(1-G5))</f>
-        <v>3.5271907320349204E-2</v>
-      </c>
-      <c r="L5" s="1">
-        <f>J5/G5</f>
-        <v>4.7712981780502255E-2</v>
-      </c>
-      <c r="M5" s="1">
-        <f>L5+K5</f>
-        <v>8.2984889100851458E-2</v>
-      </c>
-      <c r="N5" s="1">
-        <f>(I5/((1-G5)^2))-(J5/(G5^2))</f>
-        <v>0</v>
-      </c>
-      <c r="O5" s="1">
-        <f>SQRT((D5*LN(B5/(C5^2)))/E5)</f>
-        <v>0.35271907320349211</v>
-      </c>
-      <c r="P5" s="1">
-        <f>SQRT((J5/I5))</f>
-        <v>0.35271907320349205</v>
-      </c>
-      <c r="Q5" s="1">
-        <f>P5</f>
-        <v>0.35271907320349205</v>
+    <row r="5" spans="1:17" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6">
-        <v>97</v>
+        <v>10</v>
       </c>
       <c r="C6">
         <v>0.05</v>
@@ -823,38 +845,38 @@
         <v>1.5</v>
       </c>
       <c r="E6">
-        <v>462</v>
+        <v>100</v>
       </c>
       <c r="F6">
-        <v>10244</v>
+        <v>1000</v>
       </c>
       <c r="G6" s="1">
         <f>Q6/(1+Q6)</f>
-        <v>0.1562734705451784</v>
+        <v>0.26074820721510727</v>
       </c>
       <c r="H6" s="1">
         <f>1-G6</f>
-        <v>0.84372652945482163</v>
+        <v>0.73925179278489273</v>
       </c>
       <c r="I6" s="1">
         <f>E6/F6</f>
-        <v>4.509957048028114E-2</v>
+        <v>0.1</v>
       </c>
       <c r="J6" s="1">
         <f>(D6*LN(B6/(C6^2)))/F6</f>
-        <v>1.5471752526764007E-3</v>
+        <v>1.2441074460153041E-2</v>
       </c>
       <c r="K6" s="1">
         <f>I6*(G6/(1-G6))</f>
-        <v>8.3532592054494578E-3</v>
+        <v>3.5271907320349204E-2</v>
       </c>
       <c r="L6" s="1">
         <f>J6/G6</f>
-        <v>9.9004344581258581E-3</v>
+        <v>4.7712981780502255E-2</v>
       </c>
       <c r="M6" s="1">
         <f>L6+K6</f>
-        <v>1.8253693663575314E-2</v>
+        <v>8.2984889100851458E-2</v>
       </c>
       <c r="N6" s="1">
         <f>(I6/((1-G6)^2))-(J6/(G6^2))</f>
@@ -862,14 +884,78 @@
       </c>
       <c r="O6" s="1">
         <f>SQRT((D6*LN(B6/(C6^2)))/E6)</f>
-        <v>0.18521815433035552</v>
+        <v>0.35271907320349211</v>
       </c>
       <c r="P6" s="1">
         <f>SQRT((J6/I6))</f>
-        <v>0.18521815433035552</v>
+        <v>0.35271907320349205</v>
       </c>
       <c r="Q6" s="1">
         <f>P6</f>
+        <v>0.35271907320349205</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7">
+        <v>97</v>
+      </c>
+      <c r="C7">
+        <v>0.05</v>
+      </c>
+      <c r="D7">
+        <v>1.5</v>
+      </c>
+      <c r="E7">
+        <v>462</v>
+      </c>
+      <c r="F7">
+        <v>10244</v>
+      </c>
+      <c r="G7" s="1">
+        <f>Q7/(1+Q7)</f>
+        <v>0.1562734705451784</v>
+      </c>
+      <c r="H7" s="1">
+        <f>1-G7</f>
+        <v>0.84372652945482163</v>
+      </c>
+      <c r="I7" s="1">
+        <f>E7/F7</f>
+        <v>4.509957048028114E-2</v>
+      </c>
+      <c r="J7" s="1">
+        <f>(D7*LN(B7/(C7^2)))/F7</f>
+        <v>1.5471752526764007E-3</v>
+      </c>
+      <c r="K7" s="1">
+        <f>I7*(G7/(1-G7))</f>
+        <v>8.3532592054494578E-3</v>
+      </c>
+      <c r="L7" s="1">
+        <f>J7/G7</f>
+        <v>9.9004344581258581E-3</v>
+      </c>
+      <c r="M7" s="1">
+        <f>L7+K7</f>
+        <v>1.8253693663575314E-2</v>
+      </c>
+      <c r="N7" s="1">
+        <f>(I7/((1-G7)^2))-(J7/(G7^2))</f>
+        <v>0</v>
+      </c>
+      <c r="O7" s="1">
+        <f>SQRT((D7*LN(B7/(C7^2)))/E7)</f>
+        <v>0.18521815433035552</v>
+      </c>
+      <c r="P7" s="1">
+        <f>SQRT((J7/I7))</f>
+        <v>0.18521815433035552</v>
+      </c>
+      <c r="Q7" s="1">
+        <f>P7</f>
         <v>0.18521815433035552</v>
       </c>
     </row>

</xml_diff>